<commit_message>
updated the packages I want to learn
</commit_message>
<xml_diff>
--- a/resources/packages to learn.xlsx
+++ b/resources/packages to learn.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE12525-8AA7-4459-88FA-4DB478D31312}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDA2814-F585-49FA-8A8D-30D778CC67A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Practices" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Packages" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>xts</t>
   </si>
@@ -95,13 +97,139 @@
   </si>
   <si>
     <t>profvis profiler</t>
+  </si>
+  <si>
+    <t>ggrepel</t>
+  </si>
+  <si>
+    <t>ggimage</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Blog link</t>
+  </si>
+  <si>
+    <t>Time series</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Data Visualisation</t>
+  </si>
+  <si>
+    <t>General Analytics</t>
+  </si>
+  <si>
+    <t>Import/Export Files</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>caret</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/yet-another-caret-workshop/</t>
+  </si>
+  <si>
+    <t>Series Title</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Writing Better R Functions</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/writing-better-r-functions-part-four-april-17-2018/</t>
+  </si>
+  <si>
+    <t>Deep Learning from first principles</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/deep-learning-from-first-principles-in-python-r-and-octave-part-6/</t>
+  </si>
+  <si>
+    <t>Applied Economic Analysis in R</t>
+  </si>
+  <si>
+    <t>K-means clustering in R Exercises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How do I interprete AIC? </t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/how-do-i-interpret-the-aic/</t>
+  </si>
+  <si>
+    <t>Regex every R programmer should know</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Need to Read</t>
+  </si>
+  <si>
+    <t>Pimp My Rmd</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/pimp-my-rmd-a-few-tips-for-r-markdown/</t>
+  </si>
+  <si>
+    <t>Presentations</t>
+  </si>
+  <si>
+    <t>Parsing Dates and Times</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/parsing-dates-and-time-part-2-exercises/</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/regular-expressions-every-r-programmer-should-know/</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/k-means-clustering-in-r-exercises/</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/applied-economic-analysis-with-r-part-1-exercises/</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/setting-ggplot2-background-with-ggbackground/</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/</t>
+  </si>
+  <si>
+    <t>Intro to Fama French</t>
+  </si>
+  <si>
+    <t>highcharter</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/how-to-visualize-data-with-highcharter-exercises/</t>
+  </si>
+  <si>
+    <t>Descriptive Stats for variables</t>
+  </si>
+  <si>
+    <t>https://www.r-bloggers.com/get-basic-summary-statistics-for-all-the-variables-in-a-data-frame/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +245,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -126,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,15 +270,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,10 +578,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1" xr:uid="{DC5AC135-C231-4FD9-BF00-61FCBDB2D9CB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540FBFA1-88D1-4D87-A35C-396DE6FEC62F}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +765,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -471,6 +776,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -535,6 +843,162 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1AA650-A34C-4518-BAD2-95FCD0578D5E}">
+  <dimension ref="B2:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>